<commit_message>
added code to write to excel (wip)
</commit_message>
<xml_diff>
--- a/fantasy_book.xlsx
+++ b/fantasy_book.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:A5"/>
+  <dimension ref="A2:J55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -353,39 +353,1199 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="A1" t="inlineStr">
-        <is>
-          <t>Twofox</t>
-        </is>
-      </c>
-    </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Brainstorm76</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>TVTurtle</t>
+          <t>Twofox</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Tristaniac</t>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J4" t="inlineStr">
+        <is>
+          <t>Team Points</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Team SoloMid</t>
+        </is>
+      </c>
+      <c r="C5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D5" t="n">
+        <v>10</v>
+      </c>
+      <c r="E5" t="n">
+        <v>1</v>
+      </c>
+      <c r="F5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G5" t="n">
+        <v>1</v>
+      </c>
+      <c r="H5" t="n">
+        <v>0</v>
+      </c>
+      <c r="J5" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>Impact</t>
+        </is>
+      </c>
+      <c r="C7" t="n">
+        <v>3</v>
+      </c>
+      <c r="D7" t="n">
+        <v>2</v>
+      </c>
+      <c r="E7" t="n">
+        <v>8</v>
+      </c>
+      <c r="F7" t="n">
+        <v>534</v>
+      </c>
+      <c r="G7" t="n">
+        <v>22.34</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Grig</t>
+        </is>
+      </c>
+      <c r="C8" t="n">
+        <v>5</v>
+      </c>
+      <c r="D8" t="n">
+        <v>3</v>
+      </c>
+      <c r="E8" t="n">
+        <v>5</v>
+      </c>
+      <c r="F8" t="n">
+        <v>179</v>
+      </c>
+      <c r="G8" t="n">
+        <v>17.79</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Bjergsen</t>
+        </is>
+      </c>
+      <c r="C9" t="n">
+        <v>4</v>
+      </c>
+      <c r="D9" t="n">
+        <v>2</v>
+      </c>
+      <c r="E9" t="n">
+        <v>16</v>
+      </c>
+      <c r="F9" t="n">
+        <v>544</v>
+      </c>
+      <c r="G9" t="n">
+        <v>36.44</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Zven</t>
+        </is>
+      </c>
+      <c r="C10" t="n">
+        <v>9</v>
+      </c>
+      <c r="D10" t="n">
+        <v>4</v>
+      </c>
+      <c r="E10" t="n">
+        <v>10</v>
+      </c>
+      <c r="F10" t="n">
+        <v>504</v>
+      </c>
+      <c r="G10" t="n">
+        <v>36.04</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>CoreJJ</t>
+        </is>
+      </c>
+      <c r="C11" t="n">
+        <v>4</v>
+      </c>
+      <c r="D11" t="n">
+        <v>3</v>
+      </c>
+      <c r="E11" t="n">
+        <v>16</v>
+      </c>
+      <c r="F11" t="n">
+        <v>29</v>
+      </c>
+      <c r="G11" t="n">
+        <v>30.79</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Brainstorm76</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G15" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H15" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J15" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>FlyQuest</t>
+        </is>
+      </c>
+      <c r="C16" t="n">
+        <v>1</v>
+      </c>
+      <c r="D16" t="n">
+        <v>9</v>
+      </c>
+      <c r="E16" t="n">
+        <v>1</v>
+      </c>
+      <c r="F16" t="n">
+        <v>5</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0</v>
+      </c>
+      <c r="H16" t="n">
+        <v>1</v>
+      </c>
+      <c r="J16" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G17" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>Licorice</t>
+        </is>
+      </c>
+      <c r="C18" t="n">
+        <v>5</v>
+      </c>
+      <c r="D18" t="n">
+        <v>5</v>
+      </c>
+      <c r="E18" t="n">
+        <v>7</v>
+      </c>
+      <c r="F18" t="n">
+        <v>558</v>
+      </c>
+      <c r="G18" t="n">
+        <v>23.58</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>Svenskeren</t>
+        </is>
+      </c>
+      <c r="C19" t="n">
+        <v>5</v>
+      </c>
+      <c r="D19" t="n">
+        <v>6</v>
+      </c>
+      <c r="E19" t="n">
+        <v>15</v>
+      </c>
+      <c r="F19" t="n">
+        <v>363</v>
+      </c>
+      <c r="G19" t="n">
+        <v>33.13</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B20" t="inlineStr">
+        <is>
+          <t>Jensen</t>
+        </is>
+      </c>
+      <c r="C20" t="n">
+        <v>5</v>
+      </c>
+      <c r="D20" t="n">
+        <v>3</v>
+      </c>
+      <c r="E20" t="n">
+        <v>9</v>
+      </c>
+      <c r="F20" t="n">
+        <v>589</v>
+      </c>
+      <c r="G20" t="n">
+        <v>27.89</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B21" t="inlineStr">
+        <is>
+          <t>Sneaky</t>
+        </is>
+      </c>
+      <c r="C21" t="n">
+        <v>3</v>
+      </c>
+      <c r="D21" t="n">
+        <v>6</v>
+      </c>
+      <c r="E21" t="n">
+        <v>12</v>
+      </c>
+      <c r="F21" t="n">
+        <v>451</v>
+      </c>
+      <c r="G21" t="n">
+        <v>25.51</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Smoothie</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>1</v>
+      </c>
+      <c r="D22" t="n">
+        <v>3</v>
+      </c>
+      <c r="E22" t="n">
+        <v>22</v>
+      </c>
+      <c r="F22" t="n">
+        <v>41</v>
+      </c>
+      <c r="G22" t="n">
+        <v>33.91</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t>TVTurtle</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="C26" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D26" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E26" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F26" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G26" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J26" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
+      </c>
+    </row>
+    <row r="27">
+      <c r="A27" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B27" t="inlineStr">
+        <is>
+          <t>Cloud9</t>
+        </is>
+      </c>
+      <c r="C27" t="n">
+        <v>1</v>
+      </c>
+      <c r="D27" t="n">
+        <v>15</v>
+      </c>
+      <c r="E27" t="n">
+        <v>2</v>
+      </c>
+      <c r="F27" t="n">
+        <v>3</v>
+      </c>
+      <c r="G27" t="n">
+        <v>1</v>
+      </c>
+      <c r="H27" t="n">
+        <v>0</v>
+      </c>
+      <c r="J27" t="n">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="28">
+      <c r="C28" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D28" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E28" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F28" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G28" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B29" t="inlineStr">
+        <is>
+          <t>Broken Blade</t>
+        </is>
+      </c>
+      <c r="C29" t="n">
+        <v>5</v>
+      </c>
+      <c r="D29" t="n">
+        <v>6</v>
+      </c>
+      <c r="E29" t="n">
+        <v>9</v>
+      </c>
+      <c r="F29" t="n">
+        <v>471</v>
+      </c>
+      <c r="G29" t="n">
+        <v>25.21</v>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B30" t="inlineStr">
+        <is>
+          <t>Santorin</t>
+        </is>
+      </c>
+      <c r="C30" t="n">
+        <v>3</v>
+      </c>
+      <c r="D30" t="n">
+        <v>2</v>
+      </c>
+      <c r="E30" t="n">
+        <v>7</v>
+      </c>
+      <c r="F30" t="n">
+        <v>299</v>
+      </c>
+      <c r="G30" t="n">
+        <v>18.49</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Crown</t>
+        </is>
+      </c>
+      <c r="C31" t="n">
+        <v>7</v>
+      </c>
+      <c r="D31" t="n">
+        <v>1</v>
+      </c>
+      <c r="E31" t="n">
+        <v>9</v>
+      </c>
+      <c r="F31" t="n">
+        <v>625</v>
+      </c>
+      <c r="G31" t="n">
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B32" t="inlineStr">
+        <is>
+          <t>Arrow</t>
+        </is>
+      </c>
+      <c r="C32" t="n">
+        <v>5</v>
+      </c>
+      <c r="D32" t="n">
+        <v>1</v>
+      </c>
+      <c r="E32" t="n">
+        <v>8</v>
+      </c>
+      <c r="F32" t="n">
+        <v>586</v>
+      </c>
+      <c r="G32" t="n">
+        <v>27.36</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>Zeyzal</t>
+        </is>
+      </c>
+      <c r="C33" t="n">
+        <v>4</v>
+      </c>
+      <c r="D33" t="n">
+        <v>4</v>
+      </c>
+      <c r="E33" t="n">
+        <v>12</v>
+      </c>
+      <c r="F33" t="n">
+        <v>136</v>
+      </c>
+      <c r="G33" t="n">
+        <v>25.36</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Tristaniac</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J37" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>Team Liquid</t>
+        </is>
+      </c>
+      <c r="C38" t="n">
+        <v>1</v>
+      </c>
+      <c r="D38" t="n">
+        <v>14</v>
+      </c>
+      <c r="E38" t="n">
+        <v>2</v>
+      </c>
+      <c r="F38" t="n">
+        <v>5</v>
+      </c>
+      <c r="G38" t="n">
+        <v>1</v>
+      </c>
+      <c r="H38" t="n">
+        <v>0</v>
+      </c>
+      <c r="J38" t="n">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>Hauntzer</t>
+        </is>
+      </c>
+      <c r="C40" t="n">
+        <v>3</v>
+      </c>
+      <c r="D40" t="n">
+        <v>4</v>
+      </c>
+      <c r="E40" t="n">
+        <v>7</v>
+      </c>
+      <c r="F40" t="n">
+        <v>606</v>
+      </c>
+      <c r="G40" t="n">
+        <v>20.56</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>Xmithie</t>
+        </is>
+      </c>
+      <c r="C41" t="n">
+        <v>6</v>
+      </c>
+      <c r="D41" t="n">
+        <v>5</v>
+      </c>
+      <c r="E41" t="n">
+        <v>13</v>
+      </c>
+      <c r="F41" t="n">
+        <v>321</v>
+      </c>
+      <c r="G41" t="n">
+        <v>32.21</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Froggen</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>6</v>
+      </c>
+      <c r="D42" t="n">
+        <v>5</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="n">
+        <v>612</v>
+      </c>
+      <c r="G42" t="n">
+        <v>26.12</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Doublelift</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>5</v>
+      </c>
+      <c r="D43" t="n">
+        <v>2</v>
+      </c>
+      <c r="E43" t="n">
+        <v>11</v>
+      </c>
+      <c r="F43" t="n">
+        <v>693</v>
+      </c>
+      <c r="G43" t="n">
+        <v>32.43</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Big</t>
+        </is>
+      </c>
+      <c r="C44" t="n">
+        <v>0</v>
+      </c>
+      <c r="D44" t="n">
+        <v>1</v>
+      </c>
+      <c r="E44" t="n">
+        <v>13</v>
+      </c>
+      <c r="F44" t="n">
+        <v>52</v>
+      </c>
+      <c r="G44" t="n">
+        <v>19.52</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
           <t>PvtPissman</t>
         </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J48" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Team</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Golden Guardians</t>
+        </is>
+      </c>
+      <c r="C49" t="n">
+        <v>1</v>
+      </c>
+      <c r="D49" t="n">
+        <v>10</v>
+      </c>
+      <c r="E49" t="n">
+        <v>1</v>
+      </c>
+      <c r="F49" t="n">
+        <v>5</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0</v>
+      </c>
+      <c r="H49" t="n">
+        <v>0</v>
+      </c>
+      <c r="J49" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="C51" t="n">
+        <v>4</v>
+      </c>
+      <c r="D51" t="n">
+        <v>4</v>
+      </c>
+      <c r="E51" t="n">
+        <v>10</v>
+      </c>
+      <c r="F51" t="n">
+        <v>628</v>
+      </c>
+      <c r="G51" t="n">
+        <v>27.28</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Meteos</t>
+        </is>
+      </c>
+      <c r="C52" t="n">
+        <v>5</v>
+      </c>
+      <c r="D52" t="n">
+        <v>1</v>
+      </c>
+      <c r="E52" t="n">
+        <v>13</v>
+      </c>
+      <c r="F52" t="n">
+        <v>333</v>
+      </c>
+      <c r="G52" t="n">
+        <v>32.33</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>PowerOfEvil</t>
+        </is>
+      </c>
+      <c r="C53" t="n">
+        <v>4</v>
+      </c>
+      <c r="D53" t="n">
+        <v>5</v>
+      </c>
+      <c r="E53" t="n">
+        <v>6</v>
+      </c>
+      <c r="F53" t="n">
+        <v>576</v>
+      </c>
+      <c r="G53" t="n">
+        <v>20.26</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Stixxay</t>
+        </is>
+      </c>
+      <c r="C54" t="n">
+        <v>6</v>
+      </c>
+      <c r="D54" t="n">
+        <v>3</v>
+      </c>
+      <c r="E54" t="n">
+        <v>6</v>
+      </c>
+      <c r="F54" t="n">
+        <v>614</v>
+      </c>
+      <c r="G54" t="n">
+        <v>25.64</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Biofrost</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>1</v>
+      </c>
+      <c r="D55" t="n">
+        <v>3</v>
+      </c>
+      <c r="E55" t="n">
+        <v>11</v>
+      </c>
+      <c r="F55" t="n">
+        <v>29</v>
+      </c>
+      <c r="G55" t="n">
+        <v>17.29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
finished essential stat writing to excel, now formatting
</commit_message>
<xml_diff>
--- a/fantasy_book.xlsx
+++ b/fantasy_book.xlsx
@@ -345,7 +345,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A2:J55"/>
+  <dimension ref="A2:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -483,6 +483,11 @@
       <c r="G7" t="n">
         <v>22.34</v>
       </c>
+      <c r="L7" t="inlineStr">
+        <is>
+          <t>Week Total</t>
+        </is>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
@@ -592,960 +597,1265 @@
         <v>30.79</v>
       </c>
     </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Sub-1</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Nisqy</t>
+        </is>
+      </c>
+      <c r="C12" t="n">
+        <v>5</v>
+      </c>
+      <c r="D12" t="n">
+        <v>4</v>
+      </c>
+      <c r="E12" t="n">
+        <v>10</v>
+      </c>
+      <c r="F12" t="n">
+        <v>576</v>
+      </c>
+      <c r="G12" t="n">
+        <v>28.76</v>
+      </c>
+      <c r="L12" t="n">
+        <v>163.4</v>
+      </c>
+    </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
+          <t>Sub-2</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>V1per</t>
+        </is>
+      </c>
+      <c r="C13" t="n">
+        <v>3</v>
+      </c>
+      <c r="D13" t="n">
+        <v>2</v>
+      </c>
+      <c r="E13" t="n">
+        <v>5</v>
+      </c>
+      <c r="F13" t="n">
+        <v>519</v>
+      </c>
+      <c r="G13" t="n">
+        <v>17.69</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
           <t>Brainstorm76</t>
         </is>
       </c>
     </row>
-    <row r="15">
-      <c r="C15" t="inlineStr">
+    <row r="16">
+      <c r="C16" t="inlineStr">
         <is>
           <t>Wins</t>
         </is>
       </c>
-      <c r="D15" t="inlineStr">
+      <c r="D16" t="inlineStr">
         <is>
           <t>Towers</t>
         </is>
       </c>
-      <c r="E15" t="inlineStr">
+      <c r="E16" t="inlineStr">
         <is>
           <t>Barons</t>
         </is>
       </c>
-      <c r="F15" t="inlineStr">
+      <c r="F16" t="inlineStr">
         <is>
           <t>Dragons</t>
         </is>
       </c>
-      <c r="G15" t="inlineStr">
+      <c r="G16" t="inlineStr">
         <is>
           <t>Rift Heralds</t>
         </is>
       </c>
-      <c r="H15" t="inlineStr">
+      <c r="H16" t="inlineStr">
         <is>
           <t>&lt;30 Min Wins</t>
         </is>
       </c>
-      <c r="J15" t="inlineStr">
+      <c r="J16" t="inlineStr">
         <is>
           <t>Team Points</t>
         </is>
       </c>
     </row>
-    <row r="16">
-      <c r="A16" t="inlineStr">
+    <row r="17">
+      <c r="A17" t="inlineStr">
         <is>
           <t>Team</t>
         </is>
       </c>
-      <c r="B16" t="inlineStr">
+      <c r="B17" t="inlineStr">
         <is>
           <t>FlyQuest</t>
         </is>
       </c>
-      <c r="C16" t="n">
-        <v>1</v>
-      </c>
-      <c r="D16" t="n">
+      <c r="C17" t="n">
+        <v>1</v>
+      </c>
+      <c r="D17" t="n">
         <v>9</v>
       </c>
-      <c r="E16" t="n">
-        <v>1</v>
-      </c>
-      <c r="F16" t="n">
-        <v>5</v>
-      </c>
-      <c r="G16" t="n">
+      <c r="E17" t="n">
+        <v>1</v>
+      </c>
+      <c r="F17" t="n">
+        <v>5</v>
+      </c>
+      <c r="G17" t="n">
         <v>0</v>
       </c>
-      <c r="H16" t="n">
-        <v>1</v>
-      </c>
-      <c r="J16" t="n">
+      <c r="H17" t="n">
+        <v>1</v>
+      </c>
+      <c r="J17" t="n">
         <v>20</v>
       </c>
     </row>
-    <row r="17">
-      <c r="C17" t="inlineStr">
+    <row r="18">
+      <c r="C18" t="inlineStr">
         <is>
           <t>Kills</t>
         </is>
       </c>
-      <c r="D17" t="inlineStr">
+      <c r="D18" t="inlineStr">
         <is>
           <t>Deaths</t>
         </is>
       </c>
-      <c r="E17" t="inlineStr">
+      <c r="E18" t="inlineStr">
         <is>
           <t>Assists</t>
         </is>
       </c>
-      <c r="F17" t="inlineStr">
+      <c r="F18" t="inlineStr">
         <is>
           <t>CS</t>
         </is>
       </c>
-      <c r="G17" t="inlineStr">
+      <c r="G18" t="inlineStr">
         <is>
           <t>Totals</t>
         </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="inlineStr">
-        <is>
-          <t>Top</t>
-        </is>
-      </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Licorice</t>
-        </is>
-      </c>
-      <c r="C18" t="n">
-        <v>5</v>
-      </c>
-      <c r="D18" t="n">
-        <v>5</v>
-      </c>
-      <c r="E18" t="n">
-        <v>7</v>
-      </c>
-      <c r="F18" t="n">
-        <v>558</v>
-      </c>
-      <c r="G18" t="n">
-        <v>23.58</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Jungle</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Svenskeren</t>
+          <t>Licorice</t>
         </is>
       </c>
       <c r="C19" t="n">
         <v>5</v>
       </c>
       <c r="D19" t="n">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="E19" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="F19" t="n">
-        <v>363</v>
+        <v>558</v>
       </c>
       <c r="G19" t="n">
-        <v>33.13</v>
+        <v>23.58</v>
+      </c>
+      <c r="L19" t="inlineStr">
+        <is>
+          <t>Week Total</t>
+        </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>Jungle</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Jensen</t>
+          <t>Svenskeren</t>
         </is>
       </c>
       <c r="C20" t="n">
         <v>5</v>
       </c>
       <c r="D20" t="n">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="E20" t="n">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F20" t="n">
-        <v>589</v>
+        <v>363</v>
       </c>
       <c r="G20" t="n">
-        <v>27.89</v>
+        <v>33.13</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>Mid</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Sneaky</t>
+          <t>Jensen</t>
         </is>
       </c>
       <c r="C21" t="n">
+        <v>5</v>
+      </c>
+      <c r="D21" t="n">
         <v>3</v>
       </c>
-      <c r="D21" t="n">
-        <v>6</v>
-      </c>
       <c r="E21" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F21" t="n">
-        <v>451</v>
+        <v>589</v>
       </c>
       <c r="G21" t="n">
-        <v>25.51</v>
+        <v>27.89</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B22" t="inlineStr">
+        <is>
+          <t>Sneaky</t>
+        </is>
+      </c>
+      <c r="C22" t="n">
+        <v>3</v>
+      </c>
+      <c r="D22" t="n">
+        <v>6</v>
+      </c>
+      <c r="E22" t="n">
+        <v>12</v>
+      </c>
+      <c r="F22" t="n">
+        <v>451</v>
+      </c>
+      <c r="G22" t="n">
+        <v>25.51</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
           <t>Support</t>
         </is>
       </c>
-      <c r="B22" t="inlineStr">
+      <c r="B23" t="inlineStr">
         <is>
           <t>Smoothie</t>
         </is>
       </c>
-      <c r="C22" t="n">
-        <v>1</v>
-      </c>
-      <c r="D22" t="n">
+      <c r="C23" t="n">
+        <v>1</v>
+      </c>
+      <c r="D23" t="n">
         <v>3</v>
       </c>
-      <c r="E22" t="n">
+      <c r="E23" t="n">
         <v>22</v>
       </c>
-      <c r="F22" t="n">
+      <c r="F23" t="n">
         <v>41</v>
       </c>
-      <c r="G22" t="n">
+      <c r="G23" t="n">
         <v>33.91</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
+          <t>Sub-1</t>
+        </is>
+      </c>
+      <c r="B24" t="inlineStr">
+        <is>
+          <t>WildTurtle</t>
+        </is>
+      </c>
+      <c r="C24" t="n">
+        <v>4</v>
+      </c>
+      <c r="D24" t="n">
+        <v>1</v>
+      </c>
+      <c r="E24" t="n">
+        <v>3</v>
+      </c>
+      <c r="F24" t="n">
+        <v>541</v>
+      </c>
+      <c r="G24" t="n">
+        <v>17.41</v>
+      </c>
+      <c r="L24" t="n">
+        <v>164.02</v>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t>Sub-2</t>
+        </is>
+      </c>
+      <c r="B25" t="inlineStr">
+        <is>
+          <t>Olleh</t>
+        </is>
+      </c>
+      <c r="C25" t="n">
+        <v>2</v>
+      </c>
+      <c r="D25" t="n">
+        <v>5</v>
+      </c>
+      <c r="E25" t="n">
+        <v>11</v>
+      </c>
+      <c r="F25" t="n">
+        <v>115</v>
+      </c>
+      <c r="G25" t="n">
+        <v>19.15</v>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr">
+        <is>
           <t>TVTurtle</t>
         </is>
-      </c>
-    </row>
-    <row r="26">
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>Wins</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>Towers</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>Barons</t>
-        </is>
-      </c>
-      <c r="F26" t="inlineStr">
-        <is>
-          <t>Dragons</t>
-        </is>
-      </c>
-      <c r="G26" t="inlineStr">
-        <is>
-          <t>Rift Heralds</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr">
-        <is>
-          <t>&lt;30 Min Wins</t>
-        </is>
-      </c>
-      <c r="J26" t="inlineStr">
-        <is>
-          <t>Team Points</t>
-        </is>
-      </c>
-    </row>
-    <row r="27">
-      <c r="A27" t="inlineStr">
-        <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="B27" t="inlineStr">
-        <is>
-          <t>Cloud9</t>
-        </is>
-      </c>
-      <c r="C27" t="n">
-        <v>1</v>
-      </c>
-      <c r="D27" t="n">
-        <v>15</v>
-      </c>
-      <c r="E27" t="n">
-        <v>2</v>
-      </c>
-      <c r="F27" t="n">
-        <v>3</v>
-      </c>
-      <c r="G27" t="n">
-        <v>1</v>
-      </c>
-      <c r="H27" t="n">
-        <v>0</v>
-      </c>
-      <c r="J27" t="n">
-        <v>26</v>
       </c>
     </row>
     <row r="28">
       <c r="C28" t="inlineStr">
         <is>
-          <t>Kills</t>
+          <t>Wins</t>
         </is>
       </c>
       <c r="D28" t="inlineStr">
         <is>
-          <t>Deaths</t>
+          <t>Towers</t>
         </is>
       </c>
       <c r="E28" t="inlineStr">
         <is>
-          <t>Assists</t>
+          <t>Barons</t>
         </is>
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>CS</t>
+          <t>Dragons</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>Totals</t>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J28" t="inlineStr">
+        <is>
+          <t>Team Points</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Top</t>
+          <t>Team</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>Broken Blade</t>
+          <t>Cloud9</t>
         </is>
       </c>
       <c r="C29" t="n">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="D29" t="n">
-        <v>6</v>
+        <v>15</v>
       </c>
       <c r="E29" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="F29" t="n">
-        <v>471</v>
+        <v>3</v>
       </c>
       <c r="G29" t="n">
-        <v>25.21</v>
+        <v>1</v>
+      </c>
+      <c r="H29" t="n">
+        <v>0</v>
+      </c>
+      <c r="J29" t="n">
+        <v>26</v>
       </c>
     </row>
     <row r="30">
-      <c r="A30" t="inlineStr">
-        <is>
-          <t>Jungle</t>
-        </is>
-      </c>
-      <c r="B30" t="inlineStr">
-        <is>
-          <t>Santorin</t>
-        </is>
-      </c>
-      <c r="C30" t="n">
-        <v>3</v>
-      </c>
-      <c r="D30" t="n">
-        <v>2</v>
-      </c>
-      <c r="E30" t="n">
-        <v>7</v>
-      </c>
-      <c r="F30" t="n">
-        <v>299</v>
-      </c>
-      <c r="G30" t="n">
-        <v>18.49</v>
+      <c r="C30" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D30" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E30" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F30" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G30" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>Crown</t>
+          <t>Broken Blade</t>
         </is>
       </c>
       <c r="C31" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D31" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="E31" t="n">
         <v>9</v>
       </c>
       <c r="F31" t="n">
-        <v>625</v>
+        <v>471</v>
       </c>
       <c r="G31" t="n">
-        <v>33.25</v>
+        <v>25.21</v>
+      </c>
+      <c r="L31" t="inlineStr">
+        <is>
+          <t>Week Total</t>
+        </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>Jungle</t>
         </is>
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>Arrow</t>
+          <t>Santorin</t>
         </is>
       </c>
       <c r="C32" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D32" t="n">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E32" t="n">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F32" t="n">
-        <v>586</v>
+        <v>299</v>
       </c>
       <c r="G32" t="n">
-        <v>27.36</v>
+        <v>18.49</v>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Support</t>
+          <t>Mid</t>
         </is>
       </c>
       <c r="B33" t="inlineStr">
         <is>
-          <t>Zeyzal</t>
+          <t>Crown</t>
         </is>
       </c>
       <c r="C33" t="n">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="D33" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="E33" t="n">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="F33" t="n">
-        <v>136</v>
+        <v>625</v>
       </c>
       <c r="G33" t="n">
-        <v>25.36</v>
+        <v>33.25</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>Arrow</t>
+        </is>
+      </c>
+      <c r="C34" t="n">
+        <v>5</v>
+      </c>
+      <c r="D34" t="n">
+        <v>1</v>
+      </c>
+      <c r="E34" t="n">
+        <v>8</v>
+      </c>
+      <c r="F34" t="n">
+        <v>586</v>
+      </c>
+      <c r="G34" t="n">
+        <v>27.36</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Tristaniac</t>
-        </is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>Zeyzal</t>
+        </is>
+      </c>
+      <c r="C35" t="n">
+        <v>4</v>
+      </c>
+      <c r="D35" t="n">
+        <v>4</v>
+      </c>
+      <c r="E35" t="n">
+        <v>12</v>
+      </c>
+      <c r="F35" t="n">
+        <v>136</v>
+      </c>
+      <c r="G35" t="n">
+        <v>25.36</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Sub-1</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>Pobelter</t>
+        </is>
+      </c>
+      <c r="C36" t="n">
+        <v>2</v>
+      </c>
+      <c r="D36" t="n">
+        <v>4</v>
+      </c>
+      <c r="E36" t="n">
+        <v>9</v>
+      </c>
+      <c r="F36" t="n">
+        <v>477</v>
+      </c>
+      <c r="G36" t="n">
+        <v>20.27</v>
+      </c>
+      <c r="L36" t="n">
+        <v>155.67</v>
       </c>
     </row>
     <row r="37">
-      <c r="C37" t="inlineStr">
-        <is>
-          <t>Wins</t>
-        </is>
-      </c>
-      <c r="D37" t="inlineStr">
-        <is>
-          <t>Towers</t>
-        </is>
-      </c>
-      <c r="E37" t="inlineStr">
-        <is>
-          <t>Barons</t>
-        </is>
-      </c>
-      <c r="F37" t="inlineStr">
-        <is>
-          <t>Dragons</t>
-        </is>
-      </c>
-      <c r="G37" t="inlineStr">
-        <is>
-          <t>Rift Heralds</t>
-        </is>
-      </c>
-      <c r="H37" t="inlineStr">
-        <is>
-          <t>&lt;30 Min Wins</t>
-        </is>
-      </c>
-      <c r="J37" t="inlineStr">
-        <is>
-          <t>Team Points</t>
-        </is>
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Sub-2</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>Deftly</t>
+        </is>
+      </c>
+      <c r="C37" t="n">
+        <v>5</v>
+      </c>
+      <c r="D37" t="n">
+        <v>4</v>
+      </c>
+      <c r="E37" t="n">
+        <v>8</v>
+      </c>
+      <c r="F37" t="n">
+        <v>590</v>
+      </c>
+      <c r="G37" t="n">
+        <v>25.9</v>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Team</t>
-        </is>
-      </c>
-      <c r="B38" t="inlineStr">
-        <is>
-          <t>Team Liquid</t>
-        </is>
-      </c>
-      <c r="C38" t="n">
-        <v>1</v>
-      </c>
-      <c r="D38" t="n">
-        <v>14</v>
-      </c>
-      <c r="E38" t="n">
-        <v>2</v>
-      </c>
-      <c r="F38" t="n">
-        <v>5</v>
-      </c>
-      <c r="G38" t="n">
-        <v>1</v>
-      </c>
-      <c r="H38" t="n">
-        <v>0</v>
-      </c>
-      <c r="J38" t="n">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="39">
-      <c r="C39" t="inlineStr">
-        <is>
-          <t>Kills</t>
-        </is>
-      </c>
-      <c r="D39" t="inlineStr">
-        <is>
-          <t>Deaths</t>
-        </is>
-      </c>
-      <c r="E39" t="inlineStr">
-        <is>
-          <t>Assists</t>
-        </is>
-      </c>
-      <c r="F39" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G39" t="inlineStr">
-        <is>
-          <t>Totals</t>
+          <t>Tristaniac</t>
         </is>
       </c>
     </row>
     <row r="40">
-      <c r="A40" t="inlineStr">
-        <is>
-          <t>Top</t>
-        </is>
-      </c>
-      <c r="B40" t="inlineStr">
-        <is>
-          <t>Hauntzer</t>
-        </is>
-      </c>
-      <c r="C40" t="n">
-        <v>3</v>
-      </c>
-      <c r="D40" t="n">
-        <v>4</v>
-      </c>
-      <c r="E40" t="n">
-        <v>7</v>
-      </c>
-      <c r="F40" t="n">
-        <v>606</v>
-      </c>
-      <c r="G40" t="n">
-        <v>20.56</v>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J40" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>Jungle</t>
+          <t>Team</t>
         </is>
       </c>
       <c r="B41" t="inlineStr">
         <is>
-          <t>Xmithie</t>
+          <t>Team Liquid</t>
         </is>
       </c>
       <c r="C41" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D41" t="n">
-        <v>5</v>
+        <v>14</v>
       </c>
       <c r="E41" t="n">
-        <v>13</v>
+        <v>2</v>
       </c>
       <c r="F41" t="n">
-        <v>321</v>
+        <v>5</v>
       </c>
       <c r="G41" t="n">
-        <v>32.21</v>
+        <v>1</v>
+      </c>
+      <c r="H41" t="n">
+        <v>0</v>
+      </c>
+      <c r="J41" t="n">
+        <v>27</v>
       </c>
     </row>
     <row r="42">
-      <c r="A42" t="inlineStr">
-        <is>
-          <t>Mid</t>
-        </is>
-      </c>
-      <c r="B42" t="inlineStr">
-        <is>
-          <t>Froggen</t>
-        </is>
-      </c>
-      <c r="C42" t="n">
-        <v>6</v>
-      </c>
-      <c r="D42" t="n">
-        <v>5</v>
-      </c>
-      <c r="E42" t="n">
-        <v>7</v>
-      </c>
-      <c r="F42" t="n">
-        <v>612</v>
-      </c>
-      <c r="G42" t="n">
-        <v>26.12</v>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Bot</t>
+          <t>Top</t>
         </is>
       </c>
       <c r="B43" t="inlineStr">
         <is>
-          <t>Doublelift</t>
+          <t>Hauntzer</t>
         </is>
       </c>
       <c r="C43" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="D43" t="n">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="E43" t="n">
-        <v>11</v>
+        <v>7</v>
       </c>
       <c r="F43" t="n">
-        <v>693</v>
+        <v>606</v>
       </c>
       <c r="G43" t="n">
-        <v>32.43</v>
+        <v>20.56</v>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>Week Total</t>
+        </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>Support</t>
+          <t>Jungle</t>
         </is>
       </c>
       <c r="B44" t="inlineStr">
         <is>
-          <t>Big</t>
+          <t>Xmithie</t>
         </is>
       </c>
       <c r="C44" t="n">
-        <v>0</v>
+        <v>6</v>
       </c>
       <c r="D44" t="n">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="E44" t="n">
         <v>13</v>
       </c>
       <c r="F44" t="n">
-        <v>52</v>
+        <v>321</v>
       </c>
       <c r="G44" t="n">
-        <v>19.52</v>
+        <v>32.21</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Froggen</t>
+        </is>
+      </c>
+      <c r="C45" t="n">
+        <v>6</v>
+      </c>
+      <c r="D45" t="n">
+        <v>5</v>
+      </c>
+      <c r="E45" t="n">
+        <v>7</v>
+      </c>
+      <c r="F45" t="n">
+        <v>612</v>
+      </c>
+      <c r="G45" t="n">
+        <v>26.12</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>PvtPissman</t>
-        </is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Doublelift</t>
+        </is>
+      </c>
+      <c r="C46" t="n">
+        <v>5</v>
+      </c>
+      <c r="D46" t="n">
+        <v>2</v>
+      </c>
+      <c r="E46" t="n">
+        <v>11</v>
+      </c>
+      <c r="F46" t="n">
+        <v>693</v>
+      </c>
+      <c r="G46" t="n">
+        <v>32.43</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Support</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Big</t>
+        </is>
+      </c>
+      <c r="C47" t="n">
+        <v>0</v>
+      </c>
+      <c r="D47" t="n">
+        <v>1</v>
+      </c>
+      <c r="E47" t="n">
+        <v>13</v>
+      </c>
+      <c r="F47" t="n">
+        <v>52</v>
+      </c>
+      <c r="G47" t="n">
+        <v>19.52</v>
       </c>
     </row>
     <row r="48">
-      <c r="C48" t="inlineStr">
-        <is>
-          <t>Wins</t>
-        </is>
-      </c>
-      <c r="D48" t="inlineStr">
-        <is>
-          <t>Towers</t>
-        </is>
-      </c>
-      <c r="E48" t="inlineStr">
-        <is>
-          <t>Barons</t>
-        </is>
-      </c>
-      <c r="F48" t="inlineStr">
-        <is>
-          <t>Dragons</t>
-        </is>
-      </c>
-      <c r="G48" t="inlineStr">
-        <is>
-          <t>Rift Heralds</t>
-        </is>
-      </c>
-      <c r="H48" t="inlineStr">
-        <is>
-          <t>&lt;30 Min Wins</t>
-        </is>
-      </c>
-      <c r="J48" t="inlineStr">
-        <is>
-          <t>Team Points</t>
-        </is>
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Sub-1</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Ssumday</t>
+        </is>
+      </c>
+      <c r="C48" t="n">
+        <v>3</v>
+      </c>
+      <c r="D48" t="n">
+        <v>9</v>
+      </c>
+      <c r="E48" t="n">
+        <v>3</v>
+      </c>
+      <c r="F48" t="n">
+        <v>520</v>
+      </c>
+      <c r="G48" t="n">
+        <v>11.2</v>
+      </c>
+      <c r="L48" t="n">
+        <v>157.84</v>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Team</t>
+          <t>Sub-2</t>
         </is>
       </c>
       <c r="B49" t="inlineStr">
         <is>
-          <t>Golden Guardians</t>
+          <t>Goldenglue</t>
         </is>
       </c>
       <c r="C49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D49" t="n">
-        <v>10</v>
+        <v>0</v>
       </c>
       <c r="E49" t="n">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F49" t="n">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="G49" t="n">
         <v>0</v>
       </c>
-      <c r="H49" t="n">
-        <v>0</v>
-      </c>
-      <c r="J49" t="n">
-        <v>19</v>
-      </c>
     </row>
     <row r="50">
-      <c r="C50" t="inlineStr">
-        <is>
-          <t>Kills</t>
-        </is>
-      </c>
-      <c r="D50" t="inlineStr">
-        <is>
-          <t>Deaths</t>
-        </is>
-      </c>
-      <c r="E50" t="inlineStr">
-        <is>
-          <t>Assists</t>
-        </is>
-      </c>
-      <c r="F50" t="inlineStr">
-        <is>
-          <t>CS</t>
-        </is>
-      </c>
-      <c r="G50" t="inlineStr">
-        <is>
-          <t>Totals</t>
-        </is>
-      </c>
-    </row>
-    <row r="51">
-      <c r="A51" t="inlineStr">
-        <is>
-          <t>Top</t>
-        </is>
-      </c>
-      <c r="B51" t="inlineStr">
-        <is>
-          <t>Solo</t>
-        </is>
-      </c>
-      <c r="C51" t="n">
-        <v>4</v>
-      </c>
-      <c r="D51" t="n">
-        <v>4</v>
-      </c>
-      <c r="E51" t="n">
-        <v>10</v>
-      </c>
-      <c r="F51" t="n">
-        <v>628</v>
-      </c>
-      <c r="G51" t="n">
-        <v>27.28</v>
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>PvtPissman</t>
+        </is>
       </c>
     </row>
     <row r="52">
-      <c r="A52" t="inlineStr">
-        <is>
-          <t>Jungle</t>
-        </is>
-      </c>
-      <c r="B52" t="inlineStr">
-        <is>
-          <t>Meteos</t>
-        </is>
-      </c>
-      <c r="C52" t="n">
-        <v>5</v>
-      </c>
-      <c r="D52" t="n">
-        <v>1</v>
-      </c>
-      <c r="E52" t="n">
-        <v>13</v>
-      </c>
-      <c r="F52" t="n">
-        <v>333</v>
-      </c>
-      <c r="G52" t="n">
-        <v>32.33</v>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Wins</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Towers</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>Barons</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>Dragons</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>Rift Heralds</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>&lt;30 Min Wins</t>
+        </is>
+      </c>
+      <c r="J52" t="inlineStr">
+        <is>
+          <t>Team Points</t>
+        </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Mid</t>
+          <t>Team</t>
         </is>
       </c>
       <c r="B53" t="inlineStr">
         <is>
-          <t>PowerOfEvil</t>
+          <t>Golden Guardians</t>
         </is>
       </c>
       <c r="C53" t="n">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="D53" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E53" t="n">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="F53" t="n">
-        <v>576</v>
+        <v>5</v>
       </c>
       <c r="G53" t="n">
-        <v>20.26</v>
+        <v>0</v>
+      </c>
+      <c r="H53" t="n">
+        <v>0</v>
+      </c>
+      <c r="J53" t="n">
+        <v>19</v>
       </c>
     </row>
     <row r="54">
-      <c r="A54" t="inlineStr">
-        <is>
-          <t>Bot</t>
-        </is>
-      </c>
-      <c r="B54" t="inlineStr">
-        <is>
-          <t>Stixxay</t>
-        </is>
-      </c>
-      <c r="C54" t="n">
-        <v>6</v>
-      </c>
-      <c r="D54" t="n">
-        <v>3</v>
-      </c>
-      <c r="E54" t="n">
-        <v>6</v>
-      </c>
-      <c r="F54" t="n">
-        <v>614</v>
-      </c>
-      <c r="G54" t="n">
-        <v>25.64</v>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Kills</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Deaths</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>Assists</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>CS</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>Totals</t>
+        </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
+          <t>Top</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Solo</t>
+        </is>
+      </c>
+      <c r="C55" t="n">
+        <v>4</v>
+      </c>
+      <c r="D55" t="n">
+        <v>4</v>
+      </c>
+      <c r="E55" t="n">
+        <v>10</v>
+      </c>
+      <c r="F55" t="n">
+        <v>628</v>
+      </c>
+      <c r="G55" t="n">
+        <v>27.28</v>
+      </c>
+      <c r="L55" t="inlineStr">
+        <is>
+          <t>Week Total</t>
+        </is>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Jungle</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Meteos</t>
+        </is>
+      </c>
+      <c r="C56" t="n">
+        <v>5</v>
+      </c>
+      <c r="D56" t="n">
+        <v>1</v>
+      </c>
+      <c r="E56" t="n">
+        <v>13</v>
+      </c>
+      <c r="F56" t="n">
+        <v>333</v>
+      </c>
+      <c r="G56" t="n">
+        <v>32.33</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Mid</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>PowerOfEvil</t>
+        </is>
+      </c>
+      <c r="C57" t="n">
+        <v>4</v>
+      </c>
+      <c r="D57" t="n">
+        <v>5</v>
+      </c>
+      <c r="E57" t="n">
+        <v>6</v>
+      </c>
+      <c r="F57" t="n">
+        <v>576</v>
+      </c>
+      <c r="G57" t="n">
+        <v>20.26</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Bot</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Stixxay</t>
+        </is>
+      </c>
+      <c r="C58" t="n">
+        <v>6</v>
+      </c>
+      <c r="D58" t="n">
+        <v>3</v>
+      </c>
+      <c r="E58" t="n">
+        <v>6</v>
+      </c>
+      <c r="F58" t="n">
+        <v>614</v>
+      </c>
+      <c r="G58" t="n">
+        <v>25.64</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
           <t>Support</t>
         </is>
       </c>
-      <c r="B55" t="inlineStr">
+      <c r="B59" t="inlineStr">
         <is>
           <t>Biofrost</t>
         </is>
       </c>
-      <c r="C55" t="n">
-        <v>1</v>
-      </c>
-      <c r="D55" t="n">
+      <c r="C59" t="n">
+        <v>1</v>
+      </c>
+      <c r="D59" t="n">
         <v>3</v>
       </c>
-      <c r="E55" t="n">
+      <c r="E59" t="n">
         <v>11</v>
       </c>
-      <c r="F55" t="n">
+      <c r="F59" t="n">
         <v>29</v>
       </c>
-      <c r="G55" t="n">
+      <c r="G59" t="n">
         <v>17.29</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sub-1</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Contractz</t>
+        </is>
+      </c>
+      <c r="C60" t="n">
+        <v>5</v>
+      </c>
+      <c r="D60" t="n">
+        <v>3</v>
+      </c>
+      <c r="E60" t="n">
+        <v>5</v>
+      </c>
+      <c r="F60" t="n">
+        <v>337</v>
+      </c>
+      <c r="G60" t="n">
+        <v>19.37</v>
+      </c>
+      <c r="L60" t="n">
+        <v>141.8</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Sub-2</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Hakuho</t>
+        </is>
+      </c>
+      <c r="C61" t="n">
+        <v>1</v>
+      </c>
+      <c r="D61" t="n">
+        <v>6</v>
+      </c>
+      <c r="E61" t="n">
+        <v>9</v>
+      </c>
+      <c r="F61" t="n">
+        <v>105</v>
+      </c>
+      <c r="G61" t="n">
+        <v>13.55</v>
       </c>
     </row>
   </sheetData>

</xml_diff>